<commit_message>
** Update ** All features are integrated, except for noise floor.
</commit_message>
<xml_diff>
--- a/Magnetometer/Test Cases.xlsx
+++ b/Magnetometer/Test Cases.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
   <si>
     <t>Bx</t>
   </si>
@@ -648,8 +648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -951,6 +951,97 @@
         <v>13</v>
       </c>
     </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P10">
+        <f>(P2-N2)/N2 * 100</f>
+        <v>-5.101026689331202</v>
+      </c>
+      <c r="R10">
+        <f>(R2-P2)/P2 * 100</f>
+        <v>6.2444975831965337</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="P11">
+        <f t="shared" ref="P11:R16" si="0">(P3-N3)/N3 * 100</f>
+        <v>1.5768301559812018E-2</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="0"/>
+        <v>2.3218915676675445E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="0"/>
+        <v>3.560978708744094E-2</v>
+      </c>
+      <c r="R12">
+        <f t="shared" si="0"/>
+        <v>-3.3891087947385871E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="0"/>
+        <v>3.598291896749297E-2</v>
+      </c>
+      <c r="R13">
+        <f t="shared" si="0"/>
+        <v>-3.4327080590432102E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="0"/>
+        <v>-5.06716834831626</v>
+      </c>
+      <c r="R14">
+        <f t="shared" si="0"/>
+        <v>6.2081090508017711</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="0"/>
+        <v>5.7434223234311584E-2</v>
+      </c>
+      <c r="R15">
+        <f t="shared" si="0"/>
+        <v>-3.0845824990533725E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="0"/>
+        <v>4.4149771914842421E-2</v>
+      </c>
+      <c r="R16">
+        <f t="shared" si="0"/>
+        <v>-3.2864199705918695E-2</v>
+      </c>
+    </row>
     <row r="18" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I18" s="1"/>
     </row>

</xml_diff>